<commit_message>
Update feats raw data
</commit_message>
<xml_diff>
--- a/Feats.xlsx
+++ b/Feats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\projectflimflam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6F84027-6348-428A-AB10-48AC890C825C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C935DCE6-D9AD-4731-8A93-8482B4E0F4E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{52908D12-037F-4E91-9EE8-693ACF73DE32}"/>
+    <workbookView xWindow="13170" yWindow="5115" windowWidth="17970" windowHeight="15195" xr2:uid="{52908D12-037F-4E91-9EE8-693ACF73DE32}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feats" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3352" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="668">
   <si>
     <t>Further Backgrounding</t>
   </si>
@@ -3714,6 +3715,51 @@
   </si>
   <si>
     <t>Wizard</t>
+  </si>
+  <si>
+    <t>Feats</t>
+  </si>
+  <si>
+    <t>Know all the languages</t>
+  </si>
+  <si>
+    <t>Feats (Collection)</t>
+  </si>
+  <si>
+    <t>Name (Field)</t>
+  </si>
+  <si>
+    <t>Power(Field)</t>
+  </si>
+  <si>
+    <t>Tier(Field)</t>
+  </si>
+  <si>
+    <t>var featsRef = db.collection("Feats");</t>
+  </si>
+  <si>
+    <t>Class(Field)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbarian </t>
+  </si>
+  <si>
+    <t>(Document)</t>
+  </si>
+  <si>
+    <t>hashID</t>
+  </si>
+  <si>
+    <t>var query = featsRef.where("Class", "==", "Barbarian").where("Tier", "==", "Adventurer");</t>
+  </si>
+  <si>
+    <t>var query = featsRef.where("Class", "==", "Barbarian")</t>
+  </si>
+  <si>
+    <t>var query = featsRef.where("Class", "==", "General")</t>
+  </si>
+  <si>
+    <t>Union those together somehow….</t>
   </si>
 </sst>
 </file>
@@ -4108,7 +4154,7 @@
   <dimension ref="A1:D431"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10157,4 +10203,134 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8809855-2AE4-4678-9F9D-26B730DBACAC}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>